<commit_message>
Aadded the f*** space between CIS and CourseNum
</commit_message>
<xml_diff>
--- a/spreadsheets/F18original.xlsx
+++ b/spreadsheets/F18original.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="497">
   <si>
     <t>Subject</t>
   </si>
@@ -897,6 +897,9 @@
   </si>
   <si>
     <t>Prerequisite: Consent of course advisor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23</t>
   </si>
   <si>
     <t>BldgRoom</t>
@@ -26593,10 +26596,12 @@
       <c r="AZ222" s="11"/>
     </row>
     <row r="223" spans="1:256">
-      <c r="A223" s="16">
-        <v>223</v>
-      </c>
-      <c r="B223" s="17"/>
+      <c r="A223" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B223" s="17" t="s">
+        <v>290</v>
+      </c>
       <c r="C223" s="17">
         <v>23</v>
       </c>
@@ -43559,59 +43564,59 @@
   <sheetData>
     <row r="1" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A5" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -43622,19 +43627,19 @@
         <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>56</v>
@@ -43651,19 +43656,19 @@
         <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>56</v>
@@ -43674,25 +43679,25 @@
     </row>
     <row r="9" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A9" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>143</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>56</v>
@@ -43703,31 +43708,31 @@
     </row>
     <row r="10" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A10" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>56</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -43735,22 +43740,22 @@
         <v>63</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>144</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>56</v>
@@ -43764,22 +43769,22 @@
         <v>74</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>323</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>56</v>
@@ -43795,25 +43800,25 @@
     </row>
     <row r="14" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A14" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>56</v>
@@ -43824,25 +43829,25 @@
     </row>
     <row r="15" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A15" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>329</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>56</v>
@@ -43853,25 +43858,25 @@
     </row>
     <row r="16" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A16" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>56</v>
@@ -43882,25 +43887,25 @@
     </row>
     <row r="17" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A17" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>56</v>
@@ -43911,25 +43916,25 @@
     </row>
     <row r="18" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A18" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>56</v>
@@ -43940,25 +43945,25 @@
     </row>
     <row r="19" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A19" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>56</v>
@@ -43969,25 +43974,25 @@
     </row>
     <row r="20" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A20" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>56</v>
@@ -43998,25 +44003,25 @@
     </row>
     <row r="21" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A21" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>103</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>56</v>
@@ -44027,25 +44032,25 @@
     </row>
     <row r="22" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A22" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>103</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>56</v>
@@ -44056,25 +44061,25 @@
     </row>
     <row r="23" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A23" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>56</v>
@@ -44085,25 +44090,25 @@
     </row>
     <row r="24" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A24" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>127</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>56</v>
@@ -44114,25 +44119,25 @@
     </row>
     <row r="25" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A25" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>127</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>56</v>
@@ -44143,25 +44148,25 @@
     </row>
     <row r="26" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A26" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>56</v>
@@ -44172,25 +44177,25 @@
     </row>
     <row r="27" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A27" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>56</v>
@@ -44201,25 +44206,25 @@
     </row>
     <row r="28" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A28" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>56</v>
@@ -44230,30 +44235,30 @@
     </row>
     <row r="29" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A29" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="30" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A30" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>56</v>
@@ -44264,25 +44269,25 @@
     </row>
     <row r="31" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A31" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>56</v>
@@ -44293,25 +44298,25 @@
     </row>
     <row r="32" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A32" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>56</v>
@@ -44322,25 +44327,25 @@
     </row>
     <row r="33" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A33" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>56</v>
@@ -44351,25 +44356,25 @@
     </row>
     <row r="34" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A34" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>56</v>
@@ -44380,25 +44385,25 @@
     </row>
     <row r="35" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A35" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="G35" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>56</v>
@@ -44409,25 +44414,25 @@
     </row>
     <row r="36" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A36" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>56</v>
@@ -44438,25 +44443,25 @@
     </row>
     <row r="37" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A37" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>56</v>
@@ -44467,25 +44472,25 @@
     </row>
     <row r="38" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A38" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>56</v>
@@ -44496,25 +44501,25 @@
     </row>
     <row r="39" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A39" s="2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>56</v>
@@ -44525,25 +44530,25 @@
     </row>
     <row r="40" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A40" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>56</v>
@@ -44557,22 +44562,22 @@
         <v>152</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>56</v>
@@ -44583,25 +44588,25 @@
     </row>
     <row r="42" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A42" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>56</v>
@@ -44612,25 +44617,25 @@
     </row>
     <row r="43" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A43" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>56</v>
@@ -44641,25 +44646,25 @@
     </row>
     <row r="44" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A44" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>56</v>
@@ -44670,25 +44675,25 @@
     </row>
     <row r="45" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A45" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="G45" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>56</v>
@@ -44699,25 +44704,25 @@
     </row>
     <row r="46" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A46" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="G46" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>56</v>
@@ -44731,22 +44736,22 @@
         <v>256</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="G47" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>56</v>
@@ -44757,25 +44762,25 @@
     </row>
     <row r="48" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A48" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="G48" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>56</v>
@@ -44786,25 +44791,25 @@
     </row>
     <row r="49" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A49" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>133</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>56</v>
@@ -44815,25 +44820,25 @@
     </row>
     <row r="50" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A50" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>122</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>56</v>
@@ -44847,22 +44852,22 @@
         <v>248</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>56</v>
@@ -44876,22 +44881,22 @@
         <v>262</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>143</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>56</v>
@@ -44907,25 +44912,25 @@
     </row>
     <row r="54" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A54" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>133</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>56</v>
@@ -44939,22 +44944,22 @@
         <v>151</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>411</v>
-      </c>
       <c r="E55" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>143</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>56</v>
@@ -44968,22 +44973,22 @@
         <v>163</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>136</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>56</v>
@@ -44997,22 +45002,22 @@
         <v>96</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>56</v>
@@ -45026,22 +45031,22 @@
         <v>70</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>415</v>
-      </c>
       <c r="G58" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>56</v>
@@ -45055,22 +45060,22 @@
         <v>85</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>56</v>
@@ -45084,22 +45089,22 @@
         <v>109</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>56</v>
@@ -45113,22 +45118,22 @@
         <v>140</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>56</v>
@@ -45142,22 +45147,22 @@
         <v>52</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>143</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>56</v>
@@ -45176,7 +45181,7 @@
     </row>
     <row r="64" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A64" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="65" spans="1:10" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46522,13 +46527,13 @@
   <sheetData>
     <row r="1" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46536,10 +46541,10 @@
         <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46547,10 +46552,10 @@
         <v>130</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46558,10 +46563,10 @@
         <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46569,10 +46574,10 @@
         <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46580,10 +46585,10 @@
         <v>126</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46591,10 +46596,10 @@
         <v>124</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="8" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46602,10 +46607,10 @@
         <v>123</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46613,10 +46618,10 @@
         <v>121</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="10" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46624,10 +46629,10 @@
         <v>116</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46635,10 +46640,10 @@
         <v>115</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="12" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46646,10 +46651,10 @@
         <v>113</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46657,10 +46662,10 @@
         <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="14" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46668,10 +46673,10 @@
         <v>111</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="15" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46679,10 +46684,10 @@
         <v>110</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="16" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46690,10 +46695,10 @@
         <v>107</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="17" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46701,10 +46706,10 @@
         <v>106</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46712,10 +46717,10 @@
         <v>104</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46723,10 +46728,10 @@
         <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46734,10 +46739,10 @@
         <v>102</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="21" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46745,10 +46750,10 @@
         <v>101</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="22" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46756,10 +46761,10 @@
         <v>100</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46767,10 +46772,10 @@
         <v>91</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="24" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46778,10 +46783,10 @@
         <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="25" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46789,10 +46794,10 @@
         <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="26" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46800,10 +46805,10 @@
         <v>95</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="27" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46811,10 +46816,10 @@
         <v>93</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="28" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46822,10 +46827,10 @@
         <v>92</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="29" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46833,10 +46838,10 @@
         <v>89</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="30" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46844,10 +46849,10 @@
         <v>87</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="31" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46855,10 +46860,10 @@
         <v>83</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="32" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46874,10 +46879,10 @@
         <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="34" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46885,10 +46890,10 @@
         <v>78</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="35" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46896,10 +46901,10 @@
         <v>75</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="36" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46907,10 +46912,10 @@
         <v>72</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="37" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46918,10 +46923,10 @@
         <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="38" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46929,10 +46934,10 @@
         <v>66</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="39" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">
@@ -46940,10 +46945,10 @@
         <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="40" spans="1:3" customHeight="1" ht="9.75" s="1" customFormat="1">

</xml_diff>

<commit_message>
Added label tag for session numberwith calss=section
</commit_message>
<xml_diff>
--- a/spreadsheets/F18original.xlsx
+++ b/spreadsheets/F18original.xlsx
@@ -16570,14 +16570,14 @@
       <c r="AZ131" s="11"/>
     </row>
     <row r="132" spans="1:256" customHeight="1" ht="29.25">
-      <c r="A132" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B132" s="17">
-        <v>333</v>
-      </c>
-      <c r="C132" s="17" t="s">
-        <v>47</v>
+      <c r="A132" s="16">
+        <v>12</v>
+      </c>
+      <c r="B132" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C132" s="17">
+        <v>33</v>
       </c>
       <c r="D132" s="18">
         <v>3</v>
@@ -16605,11 +16605,11 @@
       <c r="O132" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="P132" s="23">
-        <v>0.54166666666667</v>
-      </c>
-      <c r="Q132" s="23">
-        <v>0.57638888888889</v>
+      <c r="P132" s="30">
+        <v>25569.083333333</v>
+      </c>
+      <c r="Q132" s="30">
+        <v>43196.576388889</v>
       </c>
       <c r="R132" s="22" t="s">
         <v>109</v>

</xml_diff>